<commit_message>
v1.1.2 release with demo project and templates
</commit_message>
<xml_diff>
--- a/ASSETS/excel/ticker/ticker_data_example.xlsx
+++ b/ASSETS/excel/ticker/ticker_data_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GC\pkg-builds\1_0_12\SPX-GC_1_0_12_win64\ASSETS\excel\ticker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GC\ASSETS\excel\ticker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D17E3F3-F46C-4376-BFE4-709C68795562}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AEE1D7-9A2B-412E-9D12-A32F6D013516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="15075" activeTab="1" xr2:uid="{D3602A80-A8D3-45A9-BF39-551D68E1E11E}"/>
+    <workbookView xWindow="14025" yWindow="1575" windowWidth="23655" windowHeight="17235" activeTab="1" xr2:uid="{D3602A80-A8D3-45A9-BF39-551D68E1E11E}"/>
   </bookViews>
   <sheets>
     <sheet name="#README" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>TICKER ITEM TEXT</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Data source is a local Excel file</t>
+  </si>
+  <si>
+    <t>This is the first news item</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -616,15 +619,14 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>

</xml_diff>